<commit_message>
ex 24 - 35
</commit_message>
<xml_diff>
--- a/Exercise summary.xlsx
+++ b/Exercise summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\git\Learn-Python-the-Hard-Way\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F438AAAB-794F-426D-97B8-DBC2B9796158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3525A4E-0EF4-4B1D-8B82-E5982D2FC1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5475" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{170A0574-5388-42CB-AC8D-D0BBEBF8E46A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{170A0574-5388-42CB-AC8D-D0BBEBF8E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Command line" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>Command line cheats</t>
   </si>
@@ -249,6 +249,39 @@
   </si>
   <si>
     <t>github</t>
+  </si>
+  <si>
+    <t>practice inc. functions</t>
+  </si>
+  <si>
+    <t>test - correcting code</t>
+  </si>
+  <si>
+    <t>logic Bool</t>
+  </si>
+  <si>
+    <t>Bool practice</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>elif</t>
+  </si>
+  <si>
+    <t>if, elif, else</t>
+  </si>
+  <si>
+    <t>for-loop</t>
+  </si>
+  <si>
+    <t>while-loop</t>
+  </si>
+  <si>
+    <t>lists</t>
+  </si>
+  <si>
+    <t>branches and functions</t>
   </si>
 </sst>
 </file>
@@ -310,13 +343,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +831,7 @@
   <dimension ref="C2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,10 +945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13672A06-5C85-4173-964C-F01A0FC6BAB8}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,12 +1106,120 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="5">
+      <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>23</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>73</v>
       </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="6">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="8">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="6">
+        <v>27</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="6">
+        <v>28</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="6">
+        <v>29</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="6">
+        <v>30</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="6">
+        <v>31</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="6">
+        <v>32</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="6">
+        <v>33</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="6">
+        <v>34</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="6">
+        <v>35</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="8">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
getting into classes and inheritence...ouch
</commit_message>
<xml_diff>
--- a/Exercise summary.xlsx
+++ b/Exercise summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\git\Learn-Python-the-Hard-Way\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB68152-4BD7-4169-AD9E-A44304862565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64C8450-CC3C-447A-9B05-42DF4A8C5E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8040" windowWidth="29040" windowHeight="15840" xr2:uid="{170A0574-5388-42CB-AC8D-D0BBEBF8E46A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{170A0574-5388-42CB-AC8D-D0BBEBF8E46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Learn Python the hard way" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
   <si>
     <t>Ex</t>
   </si>
@@ -684,6 +684,18 @@
   </si>
   <si>
     <t>exponentiates the number to the variable and sets as new variable</t>
+  </si>
+  <si>
+    <t>modules, class and objects</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>analysis and design</t>
+  </si>
+  <si>
+    <t>inheritance and compostion</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13672A06-5C85-4173-964C-F01A0FC6BAB8}">
-  <dimension ref="B2:D41"/>
+  <dimension ref="B2:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,6 +1378,78 @@
       </c>
       <c r="C41" s="5" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>